<commit_message>
excel a jour encore
</commit_message>
<xml_diff>
--- a/Metro_Arcs_Par_Station_IDs.xlsx
+++ b/Metro_Arcs_Par_Station_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noe\Documents\GitHub\ProbSciANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25780B6-33CA-439A-80FE-C4BB0E476185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C481786-6903-4AEC-B4BD-F3569373F769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="339">
   <si>
     <t>ID STATION</t>
   </si>
@@ -865,9 +865,6 @@
   </si>
   <si>
     <t>6</t>
-  </si>
-  <si>
-    <t>Sèvres - Lecourbe</t>
   </si>
   <si>
     <t>7</t>
@@ -1432,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B235" sqref="B235"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4910,8 +4907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C375"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6336,7 +6333,7 @@
         <v>110</v>
       </c>
       <c r="C129" t="s">
-        <v>276</v>
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -6344,7 +6341,7 @@
         <v>275</v>
       </c>
       <c r="B130" t="s">
-        <v>276</v>
+        <v>111</v>
       </c>
       <c r="C130" t="s">
         <v>112</v>
@@ -6539,32 +6536,32 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
+        <v>276</v>
+      </c>
+      <c r="B148" t="s">
         <v>277</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
         <v>278</v>
-      </c>
-      <c r="C148" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B149" t="s">
+        <v>278</v>
+      </c>
+      <c r="C149" t="s">
         <v>279</v>
-      </c>
-      <c r="C149" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B150" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C150" t="s">
         <v>125</v>
@@ -6572,7 +6569,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B151" t="s">
         <v>125</v>
@@ -6583,7 +6580,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B152" t="s">
         <v>126</v>
@@ -6594,7 +6591,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B153" t="s">
         <v>127</v>
@@ -6605,7 +6602,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B154" t="s">
         <v>128</v>
@@ -6616,7 +6613,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B155" t="s">
         <v>36</v>
@@ -6627,21 +6624,21 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B156" t="s">
         <v>129</v>
       </c>
       <c r="C156" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B157" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C157" t="s">
         <v>73</v>
@@ -6649,7 +6646,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B158" t="s">
         <v>73</v>
@@ -6660,7 +6657,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B159" t="s">
         <v>131</v>
@@ -6671,7 +6668,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B160" t="s">
         <v>132</v>
@@ -6682,7 +6679,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B161" t="s">
         <v>133</v>
@@ -6693,7 +6690,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B162" t="s">
         <v>134</v>
@@ -6704,7 +6701,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B163" t="s">
         <v>53</v>
@@ -6715,7 +6712,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B164" t="s">
         <v>135</v>
@@ -6726,7 +6723,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B165" t="s">
         <v>12</v>
@@ -6737,7 +6734,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B166" t="s">
         <v>136</v>
@@ -6748,21 +6745,21 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B167" t="s">
         <v>14</v>
       </c>
       <c r="C167" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B168" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C168" t="s">
         <v>138</v>
@@ -6770,7 +6767,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B169" t="s">
         <v>138</v>
@@ -6781,7 +6778,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B170" t="s">
         <v>139</v>
@@ -6792,7 +6789,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B171" t="s">
         <v>140</v>
@@ -6803,7 +6800,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B172" t="s">
         <v>141</v>
@@ -6814,7 +6811,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B173" t="s">
         <v>142</v>
@@ -6825,7 +6822,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B174" t="s">
         <v>102</v>
@@ -6836,7 +6833,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B175" t="s">
         <v>143</v>
@@ -6847,7 +6844,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B176" t="s">
         <v>144</v>
@@ -6858,7 +6855,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B177" t="s">
         <v>145</v>
@@ -6869,7 +6866,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B178" t="s">
         <v>146</v>
@@ -6880,29 +6877,29 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B179" t="s">
         <v>147</v>
       </c>
       <c r="C179" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B180" t="s">
+        <v>282</v>
+      </c>
+      <c r="C180" t="s">
         <v>283</v>
-      </c>
-      <c r="C180" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B181" t="s">
         <v>129</v>
@@ -6913,7 +6910,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B182" t="s">
         <v>37</v>
@@ -6924,7 +6921,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B183" t="s">
         <v>148</v>
@@ -6935,7 +6932,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B184" t="s">
         <v>149</v>
@@ -6946,7 +6943,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B185" t="s">
         <v>153</v>
@@ -6957,7 +6954,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B186" t="s">
         <v>150</v>
@@ -6968,7 +6965,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B187" t="s">
         <v>152</v>
@@ -6979,7 +6976,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B188" t="s">
         <v>151</v>
@@ -6990,7 +6987,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B189" t="s">
         <v>154</v>
@@ -7001,7 +6998,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B190" t="s">
         <v>155</v>
@@ -7012,7 +7009,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B191" t="s">
         <v>156</v>
@@ -7023,7 +7020,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B192" t="s">
         <v>157</v>
@@ -7034,7 +7031,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B193" t="s">
         <v>158</v>
@@ -7045,21 +7042,21 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B194" t="s">
         <v>109</v>
       </c>
       <c r="C194" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>285</v>
+      </c>
+      <c r="B195" t="s">
         <v>286</v>
-      </c>
-      <c r="B195" t="s">
-        <v>287</v>
       </c>
       <c r="C195" t="s">
         <v>160</v>
@@ -7067,7 +7064,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B196" t="s">
         <v>160</v>
@@ -7078,7 +7075,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B197" t="s">
         <v>161</v>
@@ -7089,7 +7086,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B198" t="s">
         <v>10</v>
@@ -7100,7 +7097,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B199" t="s">
         <v>162</v>
@@ -7111,7 +7108,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B200" t="s">
         <v>53</v>
@@ -7122,7 +7119,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B201" t="s">
         <v>163</v>
@@ -7133,7 +7130,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B202" t="s">
         <v>164</v>
@@ -7144,7 +7141,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B203" t="s">
         <v>165</v>
@@ -7155,7 +7152,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B204" t="s">
         <v>75</v>
@@ -7166,7 +7163,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B205" t="s">
         <v>60</v>
@@ -7177,7 +7174,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B206" t="s">
         <v>166</v>
@@ -7188,7 +7185,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B207" t="s">
         <v>167</v>
@@ -7199,7 +7196,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B208" t="s">
         <v>168</v>
@@ -7210,7 +7207,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B209" t="s">
         <v>17</v>
@@ -7221,7 +7218,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B210" t="s">
         <v>169</v>
@@ -7232,7 +7229,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B211" t="s">
         <v>170</v>
@@ -7243,7 +7240,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B212" t="s">
         <v>19</v>
@@ -7254,7 +7251,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B213" t="s">
         <v>171</v>
@@ -7265,7 +7262,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B214" t="s">
         <v>122</v>
@@ -7276,7 +7273,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B215" t="s">
         <v>172</v>
@@ -7287,7 +7284,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B216" t="s">
         <v>173</v>
@@ -7298,131 +7295,131 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B217" t="s">
         <v>174</v>
       </c>
       <c r="C217" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B218" t="s">
+        <v>287</v>
+      </c>
+      <c r="C218" t="s">
         <v>288</v>
-      </c>
-      <c r="C218" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B219" t="s">
+        <v>288</v>
+      </c>
+      <c r="C219" t="s">
         <v>289</v>
-      </c>
-      <c r="C219" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B220" t="s">
+        <v>289</v>
+      </c>
+      <c r="C220" t="s">
         <v>290</v>
-      </c>
-      <c r="C220" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B221" t="s">
+        <v>290</v>
+      </c>
+      <c r="C221" t="s">
         <v>291</v>
-      </c>
-      <c r="C221" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B222" t="s">
+        <v>291</v>
+      </c>
+      <c r="C222" t="s">
         <v>292</v>
-      </c>
-      <c r="C222" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B223" t="s">
+        <v>292</v>
+      </c>
+      <c r="C223" t="s">
         <v>293</v>
-      </c>
-      <c r="C223" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B224" t="s">
+        <v>293</v>
+      </c>
+      <c r="C224" t="s">
         <v>294</v>
-      </c>
-      <c r="C224" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B225" t="s">
+        <v>294</v>
+      </c>
+      <c r="C225" t="s">
         <v>295</v>
-      </c>
-      <c r="C225" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>296</v>
+      </c>
+      <c r="B226" t="s">
         <v>297</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>298</v>
-      </c>
-      <c r="C226" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B227" t="s">
+        <v>298</v>
+      </c>
+      <c r="C227" t="s">
         <v>299</v>
-      </c>
-      <c r="C227" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B228" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C228" t="s">
         <v>175</v>
@@ -7430,7 +7427,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B229" t="s">
         <v>175</v>
@@ -7441,7 +7438,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B230" t="s">
         <v>176</v>
@@ -7452,7 +7449,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B231" t="s">
         <v>177</v>
@@ -7463,7 +7460,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B232" t="s">
         <v>178</v>
@@ -7474,7 +7471,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B233" t="s">
         <v>179</v>
@@ -7485,7 +7482,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B234" t="s">
         <v>180</v>
@@ -7496,7 +7493,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B235" t="s">
         <v>181</v>
@@ -7507,7 +7504,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B236" t="s">
         <v>182</v>
@@ -7518,7 +7515,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B237" t="s">
         <v>105</v>
@@ -7529,7 +7526,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B238" t="s">
         <v>183</v>
@@ -7540,7 +7537,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B239" t="s">
         <v>184</v>
@@ -7551,7 +7548,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
@@ -7562,7 +7559,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B241" t="s">
         <v>185</v>
@@ -7573,7 +7570,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B242" t="s">
         <v>186</v>
@@ -7584,7 +7581,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B243" t="s">
         <v>187</v>
@@ -7595,7 +7592,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B244" t="s">
         <v>260</v>
@@ -7606,7 +7603,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B245" t="s">
         <v>134</v>
@@ -7617,7 +7614,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B246" t="s">
         <v>163</v>
@@ -7628,7 +7625,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B247" t="s">
         <v>164</v>
@@ -7639,7 +7636,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B248" t="s">
         <v>165</v>
@@ -7650,7 +7647,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B249" t="s">
         <v>75</v>
@@ -7661,7 +7658,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B250" t="s">
         <v>60</v>
@@ -7672,7 +7669,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B251" t="s">
         <v>95</v>
@@ -7683,7 +7680,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B252" t="s">
         <v>188</v>
@@ -7694,7 +7691,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B253" t="s">
         <v>189</v>
@@ -7705,7 +7702,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B254" t="s">
         <v>190</v>
@@ -7716,7 +7713,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B255" t="s">
         <v>191</v>
@@ -7727,7 +7724,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B256" t="s">
         <v>20</v>
@@ -7738,7 +7735,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B257" t="s">
         <v>192</v>
@@ -7749,7 +7746,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B258" t="s">
         <v>193</v>
@@ -7760,54 +7757,54 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B259" t="s">
         <v>194</v>
       </c>
       <c r="C259" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B260" t="s">
+        <v>300</v>
+      </c>
+      <c r="C260" t="s">
         <v>301</v>
-      </c>
-      <c r="C260" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B261" t="s">
+        <v>301</v>
+      </c>
+      <c r="C261" t="s">
         <v>302</v>
-      </c>
-      <c r="C261" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
+        <v>303</v>
+      </c>
+      <c r="B262" t="s">
         <v>304</v>
       </c>
-      <c r="B262" t="s">
+      <c r="C262" t="s">
         <v>305</v>
-      </c>
-      <c r="C262" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B263" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C263" t="s">
         <v>177</v>
@@ -7815,18 +7812,18 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B264" t="s">
         <v>207</v>
       </c>
       <c r="C264" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B265" t="s">
         <v>178</v>
@@ -7837,7 +7834,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B266" t="s">
         <v>177</v>
@@ -7848,7 +7845,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B267" t="s">
         <v>208</v>
@@ -7859,7 +7856,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B268" t="s">
         <v>205</v>
@@ -7870,7 +7867,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B269" t="s">
         <v>206</v>
@@ -7881,7 +7878,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B270" t="s">
         <v>209</v>
@@ -7892,7 +7889,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B271" t="s">
         <v>205</v>
@@ -7903,21 +7900,21 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B272" t="s">
         <v>204</v>
       </c>
       <c r="C272" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B273" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C273" t="s">
         <v>109</v>
@@ -7925,7 +7922,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B274" t="s">
         <v>109</v>
@@ -7936,7 +7933,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B275" t="s">
         <v>202</v>
@@ -7947,7 +7944,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B276" t="s">
         <v>201</v>
@@ -7958,7 +7955,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B277" t="s">
         <v>200</v>
@@ -7969,7 +7966,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B278" t="s">
         <v>199</v>
@@ -7980,7 +7977,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B279" t="s">
         <v>198</v>
@@ -7991,7 +7988,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B280" t="s">
         <v>80</v>
@@ -8002,7 +7999,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B281" t="s">
         <v>197</v>
@@ -8013,7 +8010,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B282" t="s">
         <v>196</v>
@@ -8024,7 +8021,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B283" t="s">
         <v>195</v>
@@ -8035,7 +8032,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B284" t="s">
         <v>139</v>
@@ -8046,7 +8043,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B285" t="s">
         <v>99</v>
@@ -8057,7 +8054,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B286" t="s">
         <v>119</v>
@@ -8068,7 +8065,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B287" t="s">
         <v>14</v>
@@ -8079,7 +8076,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B288" t="s">
         <v>15</v>
@@ -8090,7 +8087,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B289" t="s">
         <v>210</v>
@@ -8101,7 +8098,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B290" t="s">
         <v>58</v>
@@ -8112,7 +8109,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B291" t="s">
         <v>60</v>
@@ -8123,7 +8120,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B292" t="s">
         <v>211</v>
@@ -8134,7 +8131,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B293" t="s">
         <v>39</v>
@@ -8145,7 +8142,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B294" t="s">
         <v>212</v>
@@ -8156,7 +8153,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B295" t="s">
         <v>213</v>
@@ -8167,7 +8164,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B296" t="s">
         <v>151</v>
@@ -8178,7 +8175,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B297" t="s">
         <v>214</v>
@@ -8189,43 +8186,43 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B298" t="s">
         <v>65</v>
       </c>
       <c r="C298" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>309</v>
+      </c>
+      <c r="B299" t="s">
         <v>310</v>
       </c>
-      <c r="B299" t="s">
+      <c r="C299" t="s">
         <v>311</v>
-      </c>
-      <c r="C299" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B300" t="s">
+        <v>311</v>
+      </c>
+      <c r="C300" t="s">
         <v>312</v>
-      </c>
-      <c r="C300" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B301" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C301" t="s">
         <v>215</v>
@@ -8233,7 +8230,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B302" t="s">
         <v>215</v>
@@ -8244,7 +8241,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B303" t="s">
         <v>216</v>
@@ -8255,7 +8252,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B304" t="s">
         <v>70</v>
@@ -8266,7 +8263,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B305" t="s">
         <v>217</v>
@@ -8277,7 +8274,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B306" t="s">
         <v>218</v>
@@ -8288,7 +8285,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B307" t="s">
         <v>219</v>
@@ -8299,7 +8296,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B308" t="s">
         <v>32</v>
@@ -8310,7 +8307,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B309" t="s">
         <v>220</v>
@@ -8321,7 +8318,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B310" t="s">
         <v>221</v>
@@ -8332,7 +8329,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B311" t="s">
         <v>222</v>
@@ -8343,7 +8340,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B312" t="s">
         <v>51</v>
@@ -8354,7 +8351,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B313" t="s">
         <v>162</v>
@@ -8365,7 +8362,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B314" t="s">
         <v>10</v>
@@ -8376,7 +8373,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B315" t="s">
         <v>223</v>
@@ -8387,7 +8384,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B316" t="s">
         <v>224</v>
@@ -8398,7 +8395,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B317" t="s">
         <v>225</v>
@@ -8409,7 +8406,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B318" t="s">
         <v>199</v>
@@ -8420,21 +8417,21 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B319" t="s">
         <v>226</v>
       </c>
       <c r="C319" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B320" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C320" t="s">
         <v>84</v>
@@ -8442,7 +8439,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B321" t="s">
         <v>84</v>
@@ -8453,7 +8450,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B322" t="s">
         <v>228</v>
@@ -8464,7 +8461,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B323" t="s">
         <v>112</v>
@@ -8475,7 +8472,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B324" t="s">
         <v>229</v>
@@ -8486,7 +8483,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B325" t="s">
         <v>230</v>
@@ -8497,7 +8494,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B326" t="s">
         <v>231</v>
@@ -8508,87 +8505,87 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B327" t="s">
         <v>232</v>
       </c>
       <c r="C327" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B328" t="s">
+        <v>314</v>
+      </c>
+      <c r="C328" t="s">
         <v>315</v>
-      </c>
-      <c r="C328" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>316</v>
+      </c>
+      <c r="B329" t="s">
         <v>317</v>
       </c>
-      <c r="B329" t="s">
+      <c r="C329" t="s">
         <v>318</v>
-      </c>
-      <c r="C329" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B330" t="s">
+        <v>318</v>
+      </c>
+      <c r="C330" t="s">
         <v>319</v>
-      </c>
-      <c r="C330" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B331" t="s">
+        <v>319</v>
+      </c>
+      <c r="C331" t="s">
         <v>320</v>
-      </c>
-      <c r="C331" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B332" t="s">
+        <v>320</v>
+      </c>
+      <c r="C332" t="s">
         <v>321</v>
-      </c>
-      <c r="C332" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B333" t="s">
+        <v>321</v>
+      </c>
+      <c r="C333" t="s">
         <v>322</v>
-      </c>
-      <c r="C333" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B334" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C334" t="s">
         <v>242</v>
@@ -8596,7 +8593,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B335" t="s">
         <v>242</v>
@@ -8607,7 +8604,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B336" t="s">
         <v>241</v>
@@ -8618,7 +8615,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B337" t="s">
         <v>240</v>
@@ -8629,7 +8626,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B338" t="s">
         <v>30</v>
@@ -8640,7 +8637,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B339" t="s">
         <v>239</v>
@@ -8651,7 +8648,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B340" t="s">
         <v>51</v>
@@ -8662,21 +8659,21 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B341" t="s">
         <v>186</v>
       </c>
       <c r="C341" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B342" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C342" t="s">
         <v>161</v>
@@ -8684,7 +8681,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B343" t="s">
         <v>161</v>
@@ -8695,7 +8692,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B344" t="s">
         <v>238</v>
@@ -8706,7 +8703,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B345" t="s">
         <v>237</v>
@@ -8717,7 +8714,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B346" t="s">
         <v>201</v>
@@ -8728,10 +8725,10 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B347" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C347" t="s">
         <v>236</v>
@@ -8739,7 +8736,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B348" t="s">
         <v>236</v>
@@ -8750,7 +8747,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B349" t="s">
         <v>235</v>
@@ -8761,7 +8758,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B350" t="s">
         <v>234</v>
@@ -8772,40 +8769,40 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B351" t="s">
         <v>233</v>
       </c>
       <c r="C351" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B352" t="s">
+        <v>324</v>
+      </c>
+      <c r="C352" t="s">
         <v>325</v>
-      </c>
-      <c r="C352" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B353" t="s">
+        <v>325</v>
+      </c>
+      <c r="C353" t="s">
         <v>326</v>
-      </c>
-      <c r="C353" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B354" t="s">
         <v>243</v>
@@ -8816,7 +8813,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B355" t="s">
         <v>244</v>
@@ -8830,10 +8827,10 @@
         <v>14</v>
       </c>
       <c r="B356" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C356" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
@@ -8841,10 +8838,10 @@
         <v>14</v>
       </c>
       <c r="B357" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C357" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
@@ -8852,7 +8849,7 @@
         <v>14</v>
       </c>
       <c r="B358" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C358" t="s">
         <v>244</v>
@@ -8943,7 +8940,7 @@
         <v>120</v>
       </c>
       <c r="C366" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
@@ -8951,10 +8948,10 @@
         <v>14</v>
       </c>
       <c r="B367" t="s">
+        <v>330</v>
+      </c>
+      <c r="C367" t="s">
         <v>331</v>
-      </c>
-      <c r="C367" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
@@ -8962,7 +8959,7 @@
         <v>14</v>
       </c>
       <c r="B368" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C368" t="s">
         <v>248</v>
@@ -8987,7 +8984,7 @@
         <v>144</v>
       </c>
       <c r="C370" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
@@ -8995,10 +8992,10 @@
         <v>14</v>
       </c>
       <c r="B371" t="s">
+        <v>332</v>
+      </c>
+      <c r="C371" t="s">
         <v>333</v>
-      </c>
-      <c r="C371" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
@@ -9006,10 +9003,10 @@
         <v>14</v>
       </c>
       <c r="B372" t="s">
+        <v>333</v>
+      </c>
+      <c r="C372" t="s">
         <v>334</v>
-      </c>
-      <c r="C372" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -9017,10 +9014,10 @@
         <v>14</v>
       </c>
       <c r="B373" t="s">
+        <v>334</v>
+      </c>
+      <c r="C373" t="s">
         <v>335</v>
-      </c>
-      <c r="C373" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -9028,10 +9025,10 @@
         <v>14</v>
       </c>
       <c r="B374" t="s">
+        <v>335</v>
+      </c>
+      <c r="C374" t="s">
         <v>336</v>
-      </c>
-      <c r="C374" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
@@ -9039,10 +9036,10 @@
         <v>14</v>
       </c>
       <c r="B375" t="s">
+        <v>336</v>
+      </c>
+      <c r="C375" t="s">
         <v>337</v>
-      </c>
-      <c r="C375" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classes modif + EXCEL
</commit_message>
<xml_diff>
--- a/Metro_Arcs_Par_Station_IDs.xlsx
+++ b/Metro_Arcs_Par_Station_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noe\Documents\GitHub\ProbSciANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F5991B-8CF3-4314-8C68-D1B874C95CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84752A0E-CD93-4665-B1E8-788A9C954D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="330">
   <si>
     <t>ID STATION</t>
   </si>
@@ -1018,6 +1018,15 @@
   </si>
   <si>
     <t>Montparnasse - Bienvenue</t>
+  </si>
+  <si>
+    <t>Noms des lignes</t>
+  </si>
+  <si>
+    <t>Vitesse Moyenne train</t>
+  </si>
+  <si>
+    <t>Temps changement</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1064,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1078,13 +1087,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1391,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D247"/>
+  <dimension ref="A1:E247"/>
   <sheetViews>
-    <sheetView topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="B246" sqref="B246"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,7 +1442,7 @@
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1417,8 +1455,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1431,8 +1472,11 @@
       <c r="D2">
         <v>48.878162652696503</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1445,8 +1489,11 @@
       <c r="D3">
         <v>48.875667375651702</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1459,8 +1506,11 @@
       <c r="D4">
         <v>48.874994575222999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1473,8 +1523,11 @@
       <c r="D5">
         <v>48.872037763641003</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1488,7 +1541,7 @@
         <v>48.868724887050497</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1501,8 +1554,11 @@
       <c r="D7">
         <v>48.867656291245702</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1516,7 +1572,7 @@
         <v>48.866557992001603</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1529,8 +1585,11 @@
       <c r="D9">
         <v>48.864477838366497</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1543,8 +1602,11 @@
       <c r="D10">
         <v>48.862222264625998</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1557,8 +1619,11 @@
       <c r="D11">
         <v>48.860871211759502</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1571,8 +1636,11 @@
       <c r="D12">
         <v>48.8569534598372</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1586,7 +1654,7 @@
         <v>48.857352404237702</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1600,7 +1668,7 @@
         <v>48.8551874206563</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1614,7 +1682,7 @@
         <v>48.852054292549496</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4869,19 +4937,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C373"/>
+  <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="C283" sqref="C283"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>248</v>
       </c>
@@ -4891,8 +4962,15 @@
       <c r="C1" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -4902,8 +4980,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>251</v>
       </c>
@@ -4913,8 +4997,14 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>251</v>
       </c>
@@ -4924,8 +5014,14 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>251</v>
       </c>
@@ -4935,8 +5031,14 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>251</v>
       </c>
@@ -4946,8 +5048,14 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -4957,8 +5065,14 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>251</v>
       </c>
@@ -4968,8 +5082,14 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -4979,8 +5099,14 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4990,8 +5116,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>251</v>
       </c>
@@ -5001,8 +5133,14 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>251</v>
       </c>
@@ -5012,8 +5150,14 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>251</v>
       </c>
@@ -5023,8 +5167,14 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>251</v>
       </c>
@@ -5034,8 +5184,14 @@
       <c r="C14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>251</v>
       </c>
@@ -5045,8 +5201,14 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>251</v>
       </c>
@@ -5056,8 +5218,14 @@
       <c r="C16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>251</v>
       </c>
@@ -5067,8 +5235,14 @@
       <c r="C17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>251</v>
       </c>
@@ -5079,7 +5253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>251</v>
       </c>
@@ -5090,7 +5264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>251</v>
       </c>
@@ -5101,7 +5275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>253</v>
       </c>
@@ -5112,7 +5286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>253</v>
       </c>
@@ -5123,7 +5297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>253</v>
       </c>
@@ -5134,7 +5308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>253</v>
       </c>
@@ -5145,7 +5319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>253</v>
       </c>
@@ -5156,7 +5330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>253</v>
       </c>
@@ -5167,7 +5341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>253</v>
       </c>
@@ -5178,7 +5352,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>253</v>
       </c>
@@ -5189,7 +5363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>253</v>
       </c>
@@ -5200,7 +5374,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>253</v>
       </c>
@@ -5211,7 +5385,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5222,7 +5396,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>253</v>
       </c>
@@ -8987,5 +9161,8 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2 A6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Afficher liste et matrice adj Parfait
</commit_message>
<xml_diff>
--- a/Metro_Arcs_Par_Station_IDs.xlsx
+++ b/Metro_Arcs_Par_Station_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\ProbSciANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC39851-1962-44D0-B575-051B5AE6AFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DB6EA9-42B2-48BD-9423-0734C6B94C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="0" windowWidth="19200" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="F247" sqref="F247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>43</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>44</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>46</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>48</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>51</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>52</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>53</v>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>57</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>58</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>59</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>60</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>61</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>62</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>63</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>64</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>67</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>68</v>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>69</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>71</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>72</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>73</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>74</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>75</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>76</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>77</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>78</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>79</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>80</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>81</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>82</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>83</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>84</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>85</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>86</v>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>87</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>88</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>89</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>90</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>91</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>92</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>93</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>94</v>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>95</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>96</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>97</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>98</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>99</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>100</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>101</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>102</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>103</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>104</v>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>105</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>106</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>107</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>108</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>109</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>110</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>111</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>112</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>113</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
         <v>114</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>115</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>116</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>117</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>118</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>119</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>120</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>121</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s">
         <v>122</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s">
         <v>123</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>124</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
         <v>125</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
         <v>126</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
         <v>127</v>
@@ -3234,7 +3234,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B126" t="s">
         <v>128</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s">
         <v>129</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="B128" t="s">
         <v>130</v>
@@ -3276,7 +3276,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="B129" t="s">
         <v>131</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>132</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s">
         <v>133</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>134</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s">
         <v>135</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B134" t="s">
         <v>136</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
         <v>275</v>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>137</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
         <v>138</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
         <v>139</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
         <v>140</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
         <v>141</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
         <v>142</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s">
         <v>143</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
         <v>145</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="B145" t="s">
         <v>146</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="B146" t="s">
         <v>147</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="B147" t="s">
         <v>148</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="B148" t="s">
         <v>149</v>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="B149" t="s">
         <v>150</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="B150" t="s">
         <v>151</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="B151" t="s">
         <v>152</v>
@@ -3598,7 +3598,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
         <v>153</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>154</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>155</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>156</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="B156" t="s">
         <v>157</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="B157" t="s">
         <v>158</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="B158" t="s">
         <v>159</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="B159" t="s">
         <v>160</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>161</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="B161" t="s">
         <v>162</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="B162" t="s">
         <v>163</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="B163" t="s">
         <v>164</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>165</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="B165" t="s">
         <v>166</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="B166" t="s">
         <v>167</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B167" t="s">
         <v>168</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="B168" t="s">
         <v>169</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B169" t="s">
         <v>170</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="B170" t="s">
         <v>171</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B171" t="s">
         <v>172</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="B172" t="s">
         <v>173</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="B173" t="s">
         <v>174</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="B174" t="s">
         <v>175</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="B175" t="s">
         <v>176</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="B176" t="s">
         <v>177</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="B177" t="s">
         <v>178</v>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B178" t="s">
         <v>179</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B179" t="s">
         <v>180</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="B180" t="s">
         <v>181</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
         <v>182</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="B182" t="s">
         <v>183</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="B183" t="s">
         <v>184</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="B184" t="s">
         <v>185</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="B185" t="s">
         <v>186</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="B186" t="s">
         <v>187</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="B187" t="s">
         <v>188</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="B188" t="s">
         <v>189</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189">
-        <v>236</v>
+        <v>188</v>
       </c>
       <c r="B189" t="s">
         <v>190</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="B190" t="s">
         <v>191</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191">
-        <v>239</v>
+        <v>190</v>
       </c>
       <c r="B191" t="s">
         <v>192</v>
@@ -4158,7 +4158,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192">
-        <v>240</v>
+        <v>191</v>
       </c>
       <c r="B192" t="s">
         <v>193</v>
@@ -4172,7 +4172,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="B193" t="s">
         <v>194</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="B194" t="s">
         <v>195</v>
@@ -4200,7 +4200,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="B195" t="s">
         <v>196</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="B196" t="s">
         <v>197</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197">
-        <v>248</v>
+        <v>196</v>
       </c>
       <c r="B197" t="s">
         <v>198</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="B198" t="s">
         <v>199</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="B199" t="s">
         <v>200</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="B200" t="s">
         <v>201</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201">
-        <v>253</v>
+        <v>200</v>
       </c>
       <c r="B201" t="s">
         <v>202</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202">
-        <v>254</v>
+        <v>201</v>
       </c>
       <c r="B202" t="s">
         <v>203</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203">
-        <v>255</v>
+        <v>202</v>
       </c>
       <c r="B203" t="s">
         <v>204</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204">
-        <v>256</v>
+        <v>203</v>
       </c>
       <c r="B204" t="s">
         <v>205</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205">
-        <v>258</v>
+        <v>204</v>
       </c>
       <c r="B205" t="s">
         <v>206</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206">
-        <v>260</v>
+        <v>205</v>
       </c>
       <c r="B206" t="s">
         <v>207</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207">
-        <v>261</v>
+        <v>206</v>
       </c>
       <c r="B207" t="s">
         <v>208</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208">
-        <v>264</v>
+        <v>207</v>
       </c>
       <c r="B208" t="s">
         <v>209</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="B209" t="s">
         <v>210</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210">
-        <v>269</v>
+        <v>209</v>
       </c>
       <c r="B210" t="s">
         <v>211</v>
@@ -4424,7 +4424,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211">
-        <v>270</v>
+        <v>210</v>
       </c>
       <c r="B211" t="s">
         <v>212</v>
@@ -4438,7 +4438,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212">
-        <v>271</v>
+        <v>211</v>
       </c>
       <c r="B212" t="s">
         <v>150</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="B213" t="s">
         <v>213</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214">
-        <v>274</v>
+        <v>213</v>
       </c>
       <c r="B214" t="s">
         <v>214</v>
@@ -4480,7 +4480,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215">
-        <v>275</v>
+        <v>214</v>
       </c>
       <c r="B215" t="s">
         <v>215</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216">
-        <v>277</v>
+        <v>215</v>
       </c>
       <c r="B216" t="s">
         <v>216</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217">
-        <v>278</v>
+        <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>217</v>
@@ -4522,7 +4522,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="B218" t="s">
         <v>218</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219">
-        <v>281</v>
+        <v>218</v>
       </c>
       <c r="B219" t="s">
         <v>219</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="B220" t="s">
         <v>220</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="B221" t="s">
         <v>221</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222">
-        <v>287</v>
+        <v>221</v>
       </c>
       <c r="B222" t="s">
         <v>222</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223">
-        <v>288</v>
+        <v>222</v>
       </c>
       <c r="B223" t="s">
         <v>223</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224">
-        <v>289</v>
+        <v>223</v>
       </c>
       <c r="B224" t="s">
         <v>224</v>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225">
-        <v>291</v>
+        <v>224</v>
       </c>
       <c r="B225" t="s">
         <v>225</v>
@@ -4634,7 +4634,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226">
-        <v>292</v>
+        <v>225</v>
       </c>
       <c r="B226" t="s">
         <v>226</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227">
-        <v>294</v>
+        <v>226</v>
       </c>
       <c r="B227" t="s">
         <v>227</v>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228">
-        <v>296</v>
+        <v>227</v>
       </c>
       <c r="B228" t="s">
         <v>228</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229">
-        <v>297</v>
+        <v>228</v>
       </c>
       <c r="B229" t="s">
         <v>229</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230">
-        <v>298</v>
+        <v>229</v>
       </c>
       <c r="B230" t="s">
         <v>230</v>
@@ -4704,7 +4704,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231">
-        <v>299</v>
+        <v>230</v>
       </c>
       <c r="B231" t="s">
         <v>231</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232">
-        <v>300</v>
+        <v>231</v>
       </c>
       <c r="B232" t="s">
         <v>232</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233">
-        <v>301</v>
+        <v>232</v>
       </c>
       <c r="B233" t="s">
         <v>233</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234">
-        <v>302</v>
+        <v>233</v>
       </c>
       <c r="B234" t="s">
         <v>234</v>
@@ -4760,7 +4760,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235">
-        <v>303</v>
+        <v>234</v>
       </c>
       <c r="B235" t="s">
         <v>235</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236">
-        <v>306</v>
+        <v>235</v>
       </c>
       <c r="B236" t="s">
         <v>236</v>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237">
-        <v>307</v>
+        <v>236</v>
       </c>
       <c r="B237" t="s">
         <v>237</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238">
-        <v>312</v>
+        <v>237</v>
       </c>
       <c r="B238" t="s">
         <v>238</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239">
-        <v>314</v>
+        <v>238</v>
       </c>
       <c r="B239" t="s">
         <v>239</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240">
-        <v>315</v>
+        <v>239</v>
       </c>
       <c r="B240" t="s">
         <v>240</v>
@@ -4844,7 +4844,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241">
-        <v>316</v>
+        <v>240</v>
       </c>
       <c r="B241" t="s">
         <v>241</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242">
-        <v>318</v>
+        <v>241</v>
       </c>
       <c r="B242" t="s">
         <v>242</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="B243" t="s">
         <v>243</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244">
-        <v>321</v>
+        <v>243</v>
       </c>
       <c r="B244" t="s">
         <v>244</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245">
-        <v>328</v>
+        <v>244</v>
       </c>
       <c r="B245" t="s">
         <v>245</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246">
-        <v>329</v>
+        <v>245</v>
       </c>
       <c r="B246" t="s">
         <v>246</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247">
-        <v>330</v>
+        <v>246</v>
       </c>
       <c r="B247" t="s">
         <v>247</v>
@@ -4949,8 +4949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="F181" sqref="F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5001,7 +5001,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <f>H2/G2</f>
+        <f t="shared" ref="F2:F17" si="0">H2/G2</f>
         <v>0.55333333333333334</v>
       </c>
       <c r="G2" s="5">
@@ -5025,7 +5025,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <f>H3/G3</f>
+        <f t="shared" si="0"/>
         <v>0.496</v>
       </c>
       <c r="G3" s="5">
@@ -5049,7 +5049,7 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <f>H4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.43333333333333329</v>
       </c>
       <c r="G4" s="5">
@@ -5073,7 +5073,7 @@
         <v>269</v>
       </c>
       <c r="F5">
-        <f>H5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="G5" s="5">
@@ -5097,7 +5097,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <f>H6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.40333333333333332</v>
       </c>
       <c r="G6" s="5">
@@ -5121,7 +5121,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <f>H7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.54074074074074074</v>
       </c>
       <c r="G7" s="5">
@@ -5145,7 +5145,7 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <f>H8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.48571428571428571</v>
       </c>
       <c r="G8" s="5">
@@ -5169,7 +5169,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <f>H9/G9</f>
+        <f t="shared" si="0"/>
         <v>0.59210526315789469</v>
       </c>
       <c r="G9" s="5">
@@ -5193,7 +5193,7 @@
         <v>278</v>
       </c>
       <c r="F10">
-        <f>H10/G10</f>
+        <f t="shared" si="0"/>
         <v>0.38750000000000001</v>
       </c>
       <c r="G10" s="5">
@@ -5217,7 +5217,7 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <f>H11/G11</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="G11" s="5">
@@ -5241,7 +5241,7 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <f>H12/G12</f>
+        <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="G12" s="5">
@@ -5265,7 +5265,7 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <f>H13/G13</f>
+        <f t="shared" si="0"/>
         <v>0.46799999999999997</v>
       </c>
       <c r="G13" s="5">
@@ -5289,7 +5289,7 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <f>H14/G14</f>
+        <f t="shared" si="0"/>
         <v>0.48461538461538461</v>
       </c>
       <c r="G14" s="5">
@@ -5313,7 +5313,7 @@
         <v>12</v>
       </c>
       <c r="F15">
-        <f>H15/G15</f>
+        <f t="shared" si="0"/>
         <v>0.51724137931034486</v>
       </c>
       <c r="G15" s="5">
@@ -5337,7 +5337,7 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <f>H16/G16</f>
+        <f t="shared" si="0"/>
         <v>0.60750000000000004</v>
       </c>
       <c r="G16" s="5">
@@ -5361,7 +5361,7 @@
         <v>14</v>
       </c>
       <c r="F17">
-        <f>H17/G17</f>
+        <f t="shared" si="0"/>
         <v>0.79428571428571426</v>
       </c>
       <c r="G17" s="5">
@@ -7230,7 +7230,7 @@
         <v>278</v>
       </c>
       <c r="B185" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C185" t="s">
         <v>150</v>
@@ -7241,10 +7241,10 @@
         <v>278</v>
       </c>
       <c r="B186" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C186" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
@@ -7263,10 +7263,10 @@
         <v>278</v>
       </c>
       <c r="B188" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C188" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Graph Orienté (flèche à double sens)
</commit_message>
<xml_diff>
--- a/Metro_Arcs_Par_Station_IDs.xlsx
+++ b/Metro_Arcs_Par_Station_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\ProbSciANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD408D8A-3EC1-4F4E-92F7-D7FBD1281545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A268D07D-2E58-4199-A41C-F5EE9DA253C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="16090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="332">
   <si>
     <t>ID STATION</t>
   </si>
@@ -1015,9 +1015,6 @@
   </si>
   <si>
     <t>Aéroport d’Orly</t>
-  </si>
-  <si>
-    <t>Montparnasse - Bienvenue</t>
   </si>
   <si>
     <t>Noms des lignes</t>
@@ -1120,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1136,9 +1133,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,7 +1441,7 @@
   <dimension ref="A1:E247"/>
   <sheetViews>
     <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F247" sqref="F247"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,7 +1466,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -4955,8 +4949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D271" sqref="D271"/>
+    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D263" sqref="D263:D270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4981,20 +4975,20 @@
       <c r="C1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>332</v>
+      <c r="D1" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -9036,7 +9030,7 @@
         <v>307</v>
       </c>
       <c r="B345" t="s">
-        <v>326</v>
+        <v>84</v>
       </c>
       <c r="C345" t="s">
         <v>235</v>

</xml_diff>

<commit_message>
Excel bien à jour
</commit_message>
<xml_diff>
--- a/Metro_Arcs_Par_Station_IDs.xlsx
+++ b/Metro_Arcs_Par_Station_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\ProbSciANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8D1BB-F881-412F-96B6-75AA38267F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C5ED0-EC6C-4209-B708-C2B2F4E025AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5753,7 +5753,7 @@
   <dimension ref="A1:G252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="B250" sqref="A1:XFD1048576"/>
+      <selection activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>